<commit_message>
actualización de Entidad Relación y modelo Relacional
</commit_message>
<xml_diff>
--- a/Producto/BD/Modelo Relacional/Módelo Relacional_v1.1.xlsx
+++ b/Producto/BD/Modelo Relacional/Módelo Relacional_v1.1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
   <si>
     <t>idUsuario</t>
   </si>
@@ -54,9 +54,6 @@
     <t>fechaHoraIngreso</t>
   </si>
   <si>
-    <t>BodegaProducto</t>
-  </si>
-  <si>
     <t>idProducto</t>
   </si>
   <si>
@@ -66,15 +63,9 @@
     <t>nombreProducto</t>
   </si>
   <si>
-    <t>tipoProducto</t>
-  </si>
-  <si>
     <t>precioProducto</t>
   </si>
   <si>
-    <t>ProductoAlmacen</t>
-  </si>
-  <si>
     <t>fechaHoraSolicitud</t>
   </si>
   <si>
@@ -102,9 +93,6 @@
     <t>nombreRuta</t>
   </si>
   <si>
-    <t>AlmacenRuta</t>
-  </si>
-  <si>
     <t>idProductoAlmacenado</t>
   </si>
   <si>
@@ -177,27 +165,6 @@
     <t>correoElectronicoCliente</t>
   </si>
   <si>
-    <t>calleCliente</t>
-  </si>
-  <si>
-    <t>numeroDireccionCliente</t>
-  </si>
-  <si>
-    <t>coloniaCliente</t>
-  </si>
-  <si>
-    <t>codigoPostalCliente</t>
-  </si>
-  <si>
-    <t>estadoCliente</t>
-  </si>
-  <si>
-    <t>ciudadCliente</t>
-  </si>
-  <si>
-    <t>paisCliente</t>
-  </si>
-  <si>
     <t>idProveedor</t>
   </si>
   <si>
@@ -207,28 +174,145 @@
     <t>correoElectronicoProveedor</t>
   </si>
   <si>
-    <t>calleProveedor</t>
-  </si>
-  <si>
-    <t>numeroDireccionProveedor</t>
-  </si>
-  <si>
-    <t>coloniaProveedor</t>
-  </si>
-  <si>
-    <t>codigoPostalProveedor</t>
-  </si>
-  <si>
-    <t>estadoProveedor</t>
-  </si>
-  <si>
-    <t>ciudadProveedor</t>
-  </si>
-  <si>
-    <t>paisProveedor</t>
-  </si>
-  <si>
     <t>nombreMaterialCompra</t>
+  </si>
+  <si>
+    <t>Producción</t>
+  </si>
+  <si>
+    <t>idProductoProducción</t>
+  </si>
+  <si>
+    <t>nombreProductoProducción</t>
+  </si>
+  <si>
+    <t>tipoProductoProducción</t>
+  </si>
+  <si>
+    <t>precioProductoProducción</t>
+  </si>
+  <si>
+    <t>cantidadProductoProducción</t>
+  </si>
+  <si>
+    <t>BodegaProducción</t>
+  </si>
+  <si>
+    <t>ProducciónAlmacen</t>
+  </si>
+  <si>
+    <t>Recetas</t>
+  </si>
+  <si>
+    <t>idReceta</t>
+  </si>
+  <si>
+    <t>nombreReceta</t>
+  </si>
+  <si>
+    <t>Harina</t>
+  </si>
+  <si>
+    <t>Azúcar</t>
+  </si>
+  <si>
+    <t>Sal</t>
+  </si>
+  <si>
+    <t>Manteca</t>
+  </si>
+  <si>
+    <t>Levadura</t>
+  </si>
+  <si>
+    <t>Leche</t>
+  </si>
+  <si>
+    <t>Huevo</t>
+  </si>
+  <si>
+    <t>Cemita</t>
+  </si>
+  <si>
+    <t>Queso</t>
+  </si>
+  <si>
+    <t>MateriaPrima</t>
+  </si>
+  <si>
+    <t>idMateriaPrima</t>
+  </si>
+  <si>
+    <t>nombreMateriaPrima</t>
+  </si>
+  <si>
+    <t>valorMateriaPrima</t>
+  </si>
+  <si>
+    <t>valorProducto</t>
+  </si>
+  <si>
+    <t>Bitácora</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>responsable</t>
+  </si>
+  <si>
+    <t>acción</t>
+  </si>
+  <si>
+    <t>fechaHoraAcción</t>
+  </si>
+  <si>
+    <t>Empleado</t>
+  </si>
+  <si>
+    <t>idEmpleado</t>
+  </si>
+  <si>
+    <t>numeroTelefonoEmpleado</t>
+  </si>
+  <si>
+    <t>correoElectronicoEmpleado</t>
+  </si>
+  <si>
+    <t>calle</t>
+  </si>
+  <si>
+    <t>numeroDireccion</t>
+  </si>
+  <si>
+    <t>colonia</t>
+  </si>
+  <si>
+    <t>codigoPostal</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>ciudad</t>
+  </si>
+  <si>
+    <t>pais</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>matrículaUsuario</t>
+  </si>
+  <si>
+    <t>contraseñaUsuario</t>
+  </si>
+  <si>
+    <t>fotoUsuario</t>
+  </si>
+  <si>
+    <t>fechaNacimiento</t>
   </si>
 </sst>
 </file>
@@ -274,7 +358,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -501,22 +585,47 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color theme="0"/>
       </left>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="0"/>
       </top>
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -565,50 +674,73 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,26 +1021,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W41"/>
+  <dimension ref="A1:Y56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40:E40"/>
+    <sheetView tabSelected="1" topLeftCell="N18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y37" sqref="W37:Y37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="3"/>
     <col min="2" max="2" width="10.44140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="12" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.5546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="16.21875" style="3" customWidth="1"/>
     <col min="8" max="8" width="10.88671875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" style="3" customWidth="1"/>
     <col min="10" max="10" width="9.6640625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="3"/>
-    <col min="12" max="12" width="10" style="3" customWidth="1"/>
+    <col min="11" max="11" width="17.5546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" style="3" customWidth="1"/>
     <col min="13" max="13" width="12.88671875" style="3" customWidth="1"/>
     <col min="14" max="14" width="11.6640625" style="3" customWidth="1"/>
     <col min="15" max="15" width="8.88671875" style="3"/>
@@ -941,20 +1073,20 @@
       <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="40"/>
+      <c r="C3" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="39"/>
       <c r="E3" s="44" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="38"/>
       <c r="G3" s="38" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H3" s="38"/>
       <c r="I3" s="38" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J3" s="38"/>
       <c r="L3" s="8"/>
@@ -974,10 +1106,10 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="43"/>
+      <c r="D6" s="46"/>
       <c r="E6" s="11"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -992,10 +1124,10 @@
       <c r="D7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="40"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="7" t="s">
         <v>0</v>
       </c>
@@ -1035,7 +1167,7 @@
       <c r="K10" s="9"/>
       <c r="L10" s="33"/>
       <c r="M10" s="35" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="4"/>
@@ -1045,11 +1177,11 @@
       <c r="B11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="47" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="44"/>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="47" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="44"/>
@@ -1060,18 +1192,15 @@
       <c r="J11"/>
       <c r="L11" s="5"/>
       <c r="M11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="N11" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="O11" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="21" t="s">
-        <v>0</v>
-      </c>
+      <c r="P11" s="39"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C12" s="4"/>
@@ -1088,17 +1217,17 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
-      <c r="C14" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="41"/>
+      <c r="C14" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="40"/>
       <c r="E14" s="11"/>
       <c r="F14" s="4"/>
       <c r="G14" s="8"/>
       <c r="J14" s="12"/>
       <c r="L14" s="5"/>
       <c r="M14" s="30" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="4"/>
@@ -1110,12 +1239,12 @@
         <v>5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="40"/>
+        <v>11</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="39"/>
       <c r="G15" s="21" t="s">
         <v>0</v>
       </c>
@@ -1124,16 +1253,18 @@
       <c r="J15" s="15"/>
       <c r="L15" s="5"/>
       <c r="M15" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O15" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="8"/>
+        <v>34</v>
+      </c>
+      <c r="O15" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="M16" s="9"/>
@@ -1150,20 +1281,21 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
-      <c r="B18" s="17" t="s">
-        <v>13</v>
+      <c r="B18" s="50" t="s">
+        <v>52</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="4"/>
       <c r="L18" s="5"/>
       <c r="M18" s="32" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="4"/>
@@ -1172,47 +1304,52 @@
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
       <c r="V18" s="4"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
-      <c r="B19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="23" t="s">
-        <v>15</v>
-      </c>
+      <c r="B19" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="48"/>
+      <c r="D19" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="38"/>
       <c r="F19" s="38" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="G19" s="38"/>
-      <c r="L19" s="5"/>
+      <c r="H19" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="I19" s="38"/>
+      <c r="J19" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" s="53"/>
+      <c r="L19" s="52"/>
       <c r="M19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N19" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q19" s="39"/>
+      <c r="R19" s="39"/>
+      <c r="S19" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="N19" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="40"/>
-      <c r="S19" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="T19" s="40"/>
-      <c r="U19" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="V19" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="T19" s="60"/>
+      <c r="U19" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="V19" s="8"/>
       <c r="W19" s="8"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.3">
@@ -1222,6 +1359,10 @@
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
@@ -1230,6 +1371,7 @@
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
       <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
       <c r="V20" s="9"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.3">
@@ -1241,17 +1383,17 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B22" s="5"/>
-      <c r="C22" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="45"/>
+      <c r="C22" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="43"/>
       <c r="E22" s="6"/>
       <c r="F22" s="4"/>
       <c r="L22" s="5"/>
-      <c r="M22" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="N22" s="41"/>
+      <c r="M22" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="N22" s="40"/>
       <c r="O22" s="6"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
@@ -1259,31 +1401,33 @@
     <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B23" s="5"/>
       <c r="C23" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F23" s="38"/>
       <c r="G23" s="21" t="s">
         <v>0</v>
       </c>
       <c r="L23" s="5"/>
-      <c r="M23" s="46" t="s">
+      <c r="M23" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="N23" s="41"/>
+      <c r="O23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N23" s="46"/>
-      <c r="O23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P23" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q23" s="40"/>
-      <c r="R23" s="8"/>
+      <c r="P23" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="21" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C24" s="24"/>
@@ -1303,11 +1447,14 @@
       <c r="K25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="25" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="4"/>
@@ -1318,45 +1465,38 @@
       <c r="I26" s="4"/>
       <c r="J26" s="31"/>
       <c r="L26" s="5"/>
-      <c r="M26" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="N26" s="41"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
+      <c r="O26" s="55"/>
+      <c r="P26" s="56"/>
+      <c r="Q26" s="55"/>
+      <c r="R26" s="8"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
-      <c r="B27" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="46"/>
-      <c r="D27" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="47"/>
-      <c r="F27" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="40"/>
-      <c r="J27" s="40"/>
+      <c r="B27" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="42"/>
+      <c r="F27" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
       <c r="L27" s="5"/>
-      <c r="M27" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="N27" s="46"/>
-      <c r="O27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P27" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q27" s="40"/>
+      <c r="M27" s="57"/>
+      <c r="N27" s="57"/>
+      <c r="O27" s="59"/>
+      <c r="P27" s="58"/>
+      <c r="Q27" s="57"/>
       <c r="R27" s="8"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.3">
@@ -1375,35 +1515,72 @@
       <c r="P28" s="9"/>
       <c r="Q28" s="9"/>
     </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B29" s="4"/>
+    </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B30" s="30" t="s">
-        <v>23</v>
+      <c r="A30" s="5"/>
+      <c r="B30" s="36" t="s">
+        <v>93</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F31" s="40"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="E31" s="44"/>
+      <c r="F31" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="H31" s="65"/>
+      <c r="J31" s="64"/>
+      <c r="K31" s="64"/>
+      <c r="L31" s="64"/>
+      <c r="M31" s="64"/>
+      <c r="N31" s="64"/>
+      <c r="O31" s="64"/>
+      <c r="P31" s="8"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B32" s="4"/>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B32" s="10"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="25" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="4"/>
@@ -1426,54 +1603,54 @@
       <c r="U33" s="4"/>
       <c r="V33" s="4"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="38" t="s">
         <v>46</v>
-      </c>
-      <c r="C34" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34" s="38" t="s">
-        <v>50</v>
       </c>
       <c r="E34" s="38"/>
       <c r="F34" s="38" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G34" s="38"/>
       <c r="H34" s="38" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="I34" s="38"/>
       <c r="J34" s="38" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="K34" s="38"/>
       <c r="L34" s="38"/>
       <c r="M34" s="38" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="N34" s="38"/>
       <c r="O34" s="38" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="P34" s="38"/>
       <c r="Q34" s="38" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="R34" s="38"/>
       <c r="S34" s="38" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="T34" s="38"/>
       <c r="U34" s="38" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="V34" s="38"/>
       <c r="W34" s="8"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B35" s="10"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -1496,123 +1673,334 @@
       <c r="U35" s="9"/>
       <c r="V35" s="9"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
-      <c r="B36" s="37" t="s">
-        <v>47</v>
+      <c r="B36" s="36" t="s">
+        <v>82</v>
       </c>
       <c r="C36" s="8"/>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W36" s="4"/>
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="E37" s="38"/>
       <c r="F37" s="38" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="G37" s="38"/>
       <c r="H37" s="38" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="I37" s="38"/>
       <c r="J37" s="38" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="K37" s="38"/>
       <c r="L37" s="38"/>
       <c r="M37" s="38" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="N37" s="38"/>
       <c r="O37" s="38" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="P37" s="38"/>
       <c r="Q37" s="38" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="R37" s="38"/>
       <c r="S37" s="38" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="T37" s="38"/>
       <c r="U37" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="V37" s="38"/>
+      <c r="W37" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="X37" s="38"/>
+      <c r="Y37" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B38" s="4"/>
+      <c r="W38" s="9"/>
+      <c r="X38" s="9"/>
+      <c r="Y38" s="9"/>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A39" s="5"/>
+      <c r="B39" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="8"/>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A40" s="5"/>
+      <c r="B40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="I40" s="38"/>
+      <c r="J40" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="K40" s="38"/>
+      <c r="L40" s="38"/>
+      <c r="M40" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="N40" s="38"/>
+      <c r="O40" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="P40" s="38"/>
+      <c r="Q40" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="R40" s="38"/>
+      <c r="S40" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="T40" s="38"/>
+      <c r="U40" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="V40" s="38"/>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B41" s="10"/>
+      <c r="C41" s="9"/>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A42" s="5"/>
+      <c r="B42" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A43" s="5"/>
+      <c r="B43" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="G43" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="H43" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="I43" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="V37" s="38"/>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B38" s="4"/>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="6"/>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="49"/>
-      <c r="D40" s="50"/>
-      <c r="E40" s="51"/>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
+      <c r="J43" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="K43" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="L43" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B45" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" s="6"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="F46" s="39"/>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A48" s="5"/>
+      <c r="B48" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" s="61"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="5"/>
+      <c r="B49" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" s="48"/>
+      <c r="D49" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="E49" s="38"/>
+      <c r="F49" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="G49" s="38"/>
+      <c r="H49" s="8"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="5"/>
+      <c r="B51" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="63"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="5"/>
+      <c r="B52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="38"/>
+      <c r="E52" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="F52" s="38"/>
+      <c r="G52" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H52" s="8"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B53" s="10"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="5"/>
+      <c r="B54" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="5"/>
+      <c r="B55" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D55" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="E55" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="F55" s="38"/>
+      <c r="G55" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H55" s="8"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="52">
-    <mergeCell ref="O37:P37"/>
-    <mergeCell ref="Q37:R37"/>
-    <mergeCell ref="S37:T37"/>
-    <mergeCell ref="U37:V37"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="U34:V34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
+  <mergeCells count="75">
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="W37:X37"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="E7:F7"/>
@@ -1621,6 +2009,56 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:F11"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="U34:V34"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="S37:T37"/>
+    <mergeCell ref="U37:V37"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="O40:P40"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="U40:V40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>